<commit_message>
update files to fit the format.
</commit_message>
<xml_diff>
--- a/team14.xlsx
+++ b/team14.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F313\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\team14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4725B9-2ACC-43AA-BEBE-060EB326BECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F73E722-50B4-4ECF-B640-D434A7032A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="2265" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{1375B2CF-A2AD-4E24-9FBC-710324AF07D2}"/>
+    <workbookView xWindow="11805" yWindow="2760" windowWidth="26760" windowHeight="11385" activeTab="4" xr2:uid="{1375B2CF-A2AD-4E24-9FBC-710324AF07D2}"/>
   </bookViews>
   <sheets>
     <sheet name="開發商" sheetId="2" r:id="rId1"/>
@@ -566,15 +566,926 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>players</t>
+    <t>補充說明</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>視圖名稱</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>路由名稱</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>方法</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>路由(網址相關)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>team</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Table</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>TableSeeder</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Controller</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Developer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Game</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Request</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>Developer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>查詢所有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>遊戲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>新增</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>遊戲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料表單</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>新增</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>遊戲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>顯示單筆</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>遊戲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>修改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>遊戲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料表單</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>修改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>遊戲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>刪除</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>遊戲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>新增</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>開發商</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料表單</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>新增</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>開發商</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>顯示單筆</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>開發商</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>修改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>開發商</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料表單</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>修改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>開發商</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>刪除</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>開發商</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/store</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/{id}</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/{id}/edit</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/update/{id}</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>delete/{id}</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.store</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.show</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.edit</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.update</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.destroy</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">/create </t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/store</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/{id}</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/{id}/edit</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/update/{id}</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/delete/{id}</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.index</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
     </r>
     <r>
       <rPr>
@@ -597,7 +1508,202 @@
         <family val="1"/>
         <charset val="136"/>
       </rPr>
-      <t>players</t>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.store</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.show</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.edit</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.update</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.destroy</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>查詢所有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>開發商</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>developers</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.index</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.create</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>games</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
     </r>
     <r>
       <rPr>
@@ -612,76 +1718,12 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>players</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.index</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>players</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>補充說明</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>視圖名稱</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>路由名稱</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>方法</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>路由(網址相關)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>team</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>14</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Create</t>
-    </r>
+    <t>CreategamesTable</t>
+  </si>
+  <si>
+    <t>gamesTableSeeder</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -700,126 +1742,9 @@
         <family val="1"/>
         <charset val="136"/>
       </rPr>
-      <t>Table</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Create</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Table</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>TableSeeder</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
       <t>Controller</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>TableSeeder</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Controller</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -833,7 +1758,121 @@
         <family val="1"/>
         <charset val="136"/>
       </rPr>
-      <t>Games</t>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/show.blade.php</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>recources/views</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/index.blade.php</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>recources/views/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/form.blade.php</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>recources/views/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/edit.blade.php</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>recources/views/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>developers</t>
     </r>
     <r>
       <rPr>
@@ -859,7 +1898,85 @@
         <family val="1"/>
         <charset val="136"/>
       </rPr>
-      <t>Games</t>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/show.blade.php</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>recources/views/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/index.blade.php</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>recources/views/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>/form.blade.php</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>recources/views/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="PMingLiu"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>games</t>
     </r>
     <r>
       <rPr>
@@ -871,7 +1988,7 @@
       </rPr>
       <t>/edit.blade.php</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -885,85 +2002,7 @@
         <family val="1"/>
         <charset val="136"/>
       </rPr>
-      <t>Games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/form.blade.php</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>recources/views/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/index.blade.php</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>recources/views/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/show.blade.php</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>recources/views/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developers</t>
+      <t>games</t>
     </r>
     <r>
       <rPr>
@@ -975,1089 +2014,7 @@
       </rPr>
       <t>/create.blade.php</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>recources/views/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/edit.blade.php</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>recources/views/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/form.blade.php</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>recources/views/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/show.blade.php</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>recources/views</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/index.blade.php</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Game</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Developer</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Create</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Game</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Request</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Create</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>Developer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>查詢所有</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>遊戲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>新增</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>遊戲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料表單</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>新增</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>遊戲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>顯示單筆</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>遊戲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>修改</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>遊戲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料表單</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>修改</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>遊戲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>刪除</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>遊戲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>新增</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>開發商</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料表單</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>新增</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>開發商</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>顯示單筆</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>開發商</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>修改</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>開發商</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料表單</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>修改</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>開發商</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>刪除</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>開發商</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/store</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/{id}</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/{id}/edit</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/update/{id}</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>delete/{id}</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.store</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.show</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.edit</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.update</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.destroy</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t xml:space="preserve">/create </t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/store</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/{id}</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/{id}/edit</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/update/{id}</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>/delete/{id}</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.index</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.create</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.store</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.show</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.edit</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.update</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.destroy</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>查詢所有</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>開發商</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="PMingLiu"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>developers</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3660,8 +3617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5607F317-6968-4BD5-91AF-EA5089F7CA64}">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4012,8 +3969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DA4D13-CDDB-4388-A7A2-ED9B9BB868C1}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4043,7 +4000,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>121</v>
@@ -4071,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>107</v>
@@ -4085,7 +4042,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>107</v>
@@ -4113,7 +4070,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>107</v>
@@ -4127,7 +4084,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>107</v>
@@ -4155,7 +4112,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>116</v>
@@ -4169,7 +4126,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>116</v>
@@ -4200,7 +4157,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>107</v>
@@ -4214,7 +4171,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>107</v>
@@ -4242,7 +4199,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>113</v>
@@ -4256,7 +4213,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>113</v>
@@ -4284,7 +4241,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>107</v>
@@ -4298,7 +4255,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>107</v>
@@ -4312,7 +4269,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>148</v>
+        <v>195</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>107</v>
@@ -4326,7 +4283,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>107</v>
@@ -4340,7 +4297,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>107</v>
@@ -4354,7 +4311,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>107</v>
@@ -4368,7 +4325,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>107</v>
@@ -4382,7 +4339,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>107</v>
@@ -4396,7 +4353,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>107</v>
@@ -4410,7 +4367,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>107</v>
@@ -4432,8 +4389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A70A90-0AD6-42B0-9A9A-6494859CFF3E}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4448,57 +4405,57 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1">
       <c r="A1" s="47" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="44" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>132</v>
+        <v>183</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>127</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="14" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>130</v>
+        <v>184</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>126</v>
@@ -4506,16 +4463,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="14" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>128</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="27" t="s">
@@ -4524,37 +4481,37 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="40" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>127</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="F5" s="37"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="14" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>126</v>
@@ -4562,16 +4519,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="14" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>125</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="27" t="s">
@@ -4580,53 +4537,53 @@
     </row>
     <row r="8" spans="1:6" ht="17.25" thickBot="1">
       <c r="A8" s="11" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>123</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="36" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>127</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="F9" s="32"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="14" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>126</v>
@@ -4634,16 +4591,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="14" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>128</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="E11" s="28"/>
       <c r="F11" s="27" t="s">
@@ -4652,37 +4609,37 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="31" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="14" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>126</v>
@@ -4690,16 +4647,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="14" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>125</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="27" t="s">
@@ -4708,16 +4665,16 @@
     </row>
     <row r="15" spans="1:6" ht="17.25" thickBot="1">
       <c r="A15" s="11" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>123</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="24"/>

</xml_diff>

<commit_message>
add update, create ,store function. d_id is now fillable. section game_contents->game_content developer and game form is done. reformating the code. index order by id.
</commit_message>
<xml_diff>
--- a/team14.xlsx
+++ b/team14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\team14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063418DA-CE76-4BC7-AE1B-A17F5CAA9964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64C2CE5-D3B5-4C46-84D2-B2BFA51E1178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15150" yWindow="2565" windowWidth="26760" windowHeight="11385" activeTab="3" xr2:uid="{1375B2CF-A2AD-4E24-9FBC-710324AF07D2}"/>
+    <workbookView xWindow="15150" yWindow="2565" windowWidth="26760" windowHeight="11385" activeTab="4" xr2:uid="{1375B2CF-A2AD-4E24-9FBC-710324AF07D2}"/>
   </bookViews>
   <sheets>
     <sheet name="開發商" sheetId="2" r:id="rId1"/>
@@ -3861,7 +3861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66809FF1-8E0E-4352-9D91-4DF966DF14C0}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -4012,8 +4012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DA4D13-CDDB-4388-A7A2-ED9B9BB868C1}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>